<commit_message>
update ketquaDAO và QuanLiDiemHocSinhDAO
</commit_message>
<xml_diff>
--- a/DCT1201.xlsx
+++ b/DCT1201.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Tổng số học sinh:</t>
   </si>
   <si>
-    <t>4</t>
+    <t>2</t>
   </si>
   <si>
     <t>Số lượng hoc sinh khá:</t>
@@ -29,15 +29,9 @@
     <t>Số lượng học sinh giỏi:</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Số lượng học sinh trung bình:</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Số lượng học sinh yếu:</t>
   </si>
   <si>
@@ -56,49 +50,28 @@
     <t>HỌC LỰC</t>
   </si>
   <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>Đặng Huỳnh</t>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Quang</t>
   </si>
   <si>
     <t>DCT1201</t>
   </si>
   <si>
+    <t>8.58</t>
+  </si>
+  <si>
+    <t>Giỏi</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Đặng Huỳnh Như Y</t>
+  </si>
+  <si>
     <t>8.5</t>
-  </si>
-  <si>
-    <t>Giỏi</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Quang</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>Đặng Huỳnh Như Y</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Nhã</t>
-  </si>
-  <si>
-    <t>5.83333</t>
-  </si>
-  <si>
-    <t>Trung bình</t>
   </si>
 </sst>
 </file>
@@ -143,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -170,20 +143,20 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -191,87 +164,53 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>